<commit_message>
material: Add 'todo' comment to the print inventory.
</commit_message>
<xml_diff>
--- a/material/cards/print_inventory.xlsx
+++ b/material/cards/print_inventory.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="11">
   <si>
     <t>l</t>
   </si>
@@ -55,12 +55,15 @@
   <si>
     <t>only in even</t>
   </si>
+  <si>
+    <t>todo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,8 +71,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,8 +111,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -165,11 +193,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -220,8 +264,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Notiz" xfId="1" builtinId="10"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,7 +554,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,6 +790,15 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="D17" s="4" t="s">
         <v>1</v>
       </c>
@@ -980,5 +1040,6 @@
     <sortCondition ref="B20:B39"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update card print files; .gitignore; inventory
remove superfluous print files, update inventory as all cards printed
</commit_message>
<xml_diff>
--- a/material/cards/print_inventory.xlsx
+++ b/material/cards/print_inventory.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="14">
   <si>
     <t>l</t>
   </si>
@@ -67,9 +67,6 @@
   <si>
     <t>required inventory</t>
   </si>
-  <si>
-    <t>printed</t>
-  </si>
 </sst>
 </file>
 
@@ -106,7 +103,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,12 +113,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,18 +164,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -476,7 +466,7 @@
   <dimension ref="A1:S55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,18 +477,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -535,13 +525,13 @@
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -557,27 +547,27 @@
         <v>11</v>
       </c>
       <c r="J4" s="1"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -593,27 +583,27 @@
         <v>11</v>
       </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -623,27 +613,27 @@
         <v>11</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -653,27 +643,27 @@
         <v>11</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -686,27 +676,27 @@
         <v>11</v>
       </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -719,27 +709,27 @@
         <v>11</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="8"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -752,27 +742,27 @@
         <v>11</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="8"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -785,27 +775,27 @@
         <v>11</v>
       </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="8"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="4"/>
@@ -813,30 +803,30 @@
         <v>11</v>
       </c>
       <c r="H12" s="4"/>
-      <c r="I12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="8"/>
+      <c r="I12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="4"/>
@@ -844,30 +834,30 @@
         <v>11</v>
       </c>
       <c r="H13" s="4"/>
-      <c r="I13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="8"/>
+      <c r="I13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="7"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="4"/>
@@ -875,30 +865,30 @@
         <v>11</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="I14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="8"/>
+      <c r="I14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="7"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="4" t="s">
@@ -914,27 +904,27 @@
         <v>11</v>
       </c>
       <c r="J15" s="4"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="8"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="7"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>0</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -948,27 +938,27 @@
         <v>11</v>
       </c>
       <c r="J16" s="4"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="8"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="7"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>0</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -982,27 +972,27 @@
         <v>11</v>
       </c>
       <c r="J17" s="4"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="8"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="7"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>0</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -1016,28 +1006,28 @@
         <v>11</v>
       </c>
       <c r="J18" s="4"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="8"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="7"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>0</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -1049,21 +1039,21 @@
         <v>11</v>
       </c>
       <c r="J19" s="4"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="8"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="7"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -1075,15 +1065,15 @@
         <v>11</v>
       </c>
       <c r="J20" s="4"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="8"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="7"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
@@ -1092,7 +1082,7 @@
       <c r="D21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="4" t="s">
@@ -1106,27 +1096,27 @@
         <v>11</v>
       </c>
       <c r="J21" s="4"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="8"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="7"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -1140,27 +1130,27 @@
         <v>11</v>
       </c>
       <c r="J22" s="4"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="8"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="7"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -1174,27 +1164,27 @@
         <v>11</v>
       </c>
       <c r="J23" s="4"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="8"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="7"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -1210,27 +1200,27 @@
         <v>11</v>
       </c>
       <c r="J24" s="4"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="8"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="7"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -1246,27 +1236,27 @@
         <v>11</v>
       </c>
       <c r="J25" s="4"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="8"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F26" s="4" t="s">
@@ -1282,27 +1272,27 @@
         <v>11</v>
       </c>
       <c r="J26" s="4"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="8"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="7"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -1314,222 +1304,222 @@
       <c r="H27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I27" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K27" s="8"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="8"/>
+      <c r="I27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="7"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="7"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K28" s="8"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="8"/>
+      <c r="B28" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" s="7"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="7"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K29" s="8"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="8"/>
+      <c r="B29" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="7"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="7"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K30" s="8"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="8"/>
+      <c r="B30" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K30" s="7"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="7"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K31" s="8"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
+      <c r="B31" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K31" s="7"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
+      <c r="B32" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
+      <c r="B33" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
+      <c r="B34" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
+      <c r="B35" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
+      <c r="B36" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
+      <c r="B37" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="4"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1537,7 +1527,7 @@
       <c r="A41" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1545,7 +1535,7 @@
       <c r="A42" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1553,7 +1543,7 @@
       <c r="A43" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1561,7 +1551,7 @@
       <c r="A44" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1569,7 +1559,7 @@
       <c r="A45" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1577,7 +1567,7 @@
       <c r="A46" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1585,7 +1575,7 @@
       <c r="A47" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1593,7 +1583,7 @@
       <c r="A48" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1601,7 +1591,7 @@
       <c r="A49" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1609,7 +1599,7 @@
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1617,7 +1607,7 @@
       <c r="A51" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1625,7 +1615,7 @@
       <c r="A52" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1633,7 +1623,7 @@
       <c r="A53" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1641,7 +1631,7 @@
       <c r="A54" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1649,7 +1639,7 @@
       <c r="A55" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="10" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update procedure (copy from overleaf); update inventory; PowerPoint files
</commit_message>
<xml_diff>
--- a/material/cards/print_inventory.xlsx
+++ b/material/cards/print_inventory.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="15">
   <si>
     <t>l</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>required inventory</t>
+  </si>
+  <si>
+    <t>familiarization</t>
   </si>
 </sst>
 </file>
@@ -466,14 +469,14 @@
   <dimension ref="A1:S55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="11.5546875" style="1"/>
     <col min="4" max="8" width="5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.109375" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -501,12 +504,15 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -543,12 +549,10 @@
       <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -579,12 +583,10 @@
       <c r="H5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
@@ -606,15 +608,14 @@
       <c r="E6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
@@ -636,15 +637,13 @@
       <c r="E7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
@@ -669,15 +668,13 @@
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K8" s="7"/>
-      <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -705,12 +702,10 @@
       <c r="H9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K9" s="7"/>
-      <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -738,12 +733,10 @@
       <c r="H10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K10" s="7"/>
-      <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -771,12 +764,10 @@
       <c r="H11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K11" s="7"/>
-      <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -799,15 +790,17 @@
         <v>1</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="I12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K12" s="7"/>
-      <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
@@ -830,15 +823,14 @@
         <v>1</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4" t="s">
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K13" s="7"/>
-      <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
@@ -861,15 +853,14 @@
         <v>1</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4" t="s">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K14" s="7"/>
-      <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
@@ -900,12 +891,10 @@
       <c r="H15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="4"/>
+      <c r="J15" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K15" s="7"/>
-      <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
@@ -930,16 +919,14 @@
       <c r="F16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="J16" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K16" s="7"/>
-      <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
@@ -964,16 +951,14 @@
       <c r="F17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="J17" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K17" s="7"/>
-      <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
@@ -998,16 +983,14 @@
       <c r="F18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K18" s="7"/>
-      <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
@@ -1036,11 +1019,12 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K19" s="7"/>
-      <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
@@ -1061,12 +1045,10 @@
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="4"/>
+      <c r="J20" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K20" s="7"/>
-      <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
@@ -1088,16 +1070,15 @@
       <c r="F21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="I21" s="4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
@@ -1122,16 +1103,17 @@
       <c r="F22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="I22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K22" s="7"/>
-      <c r="L22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8"/>
@@ -1156,16 +1138,14 @@
       <c r="F23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K23" s="7"/>
-      <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
@@ -1196,12 +1176,10 @@
       <c r="H24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="4"/>
+      <c r="J24" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
@@ -1232,12 +1210,10 @@
       <c r="H25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J25" s="4"/>
+      <c r="J25" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K25" s="7"/>
-      <c r="L25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
@@ -1268,12 +1244,10 @@
       <c r="H26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J26" s="4"/>
+      <c r="J26" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K26" s="7"/>
-      <c r="L26" s="8"/>
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
@@ -1304,11 +1278,10 @@
       <c r="H27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="J27" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K27" s="7"/>
-      <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>

</xml_diff>